<commit_message>
Richiesta accreditamento per A1#200000SWHSHARK/e-Shark S.r.l./FaithK/2.9.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#200000SWHSHARK/e-Shark S.r.l/FaithK/2.9.0/report-checklist.xlsx
+++ b/GATEWAY/A1#200000SWHSHARK/e-Shark S.r.l/FaithK/2.9.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\it-fse-accreditamento\GATEWAY\A1#200000SWHSHARK\e-Shark S.r.l\FaithK\2.9.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E706F3B-D782-4798-A5A6-E09A395B1C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4C7576-8C32-45EB-835C-F8C3912D09DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1650" windowWidth="29010" windowHeight="14610" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4700,16 +4700,16 @@
     <t>Il campo è un dato obbligatorio, non è quindi possibile replicare l'errore.</t>
   </si>
   <si>
-    <t>2024-01-02 14:20:37Z</t>
-  </si>
-  <si>
-    <t>2717ab0e53990e25</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.28ea7a16ff81da547412820fd54840002a5a2255050e7132e2bf4ab2172e5f4d.218150a800^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Non è possibile replicare la condizione in quanto la capacità motoria è un campo obbligatorio in fase di inserimento.</t>
+  </si>
+  <si>
+    <t>2024-01-18 10:22:00Z</t>
+  </si>
+  <si>
+    <t>43e9fbb5ce14e6ac</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.406f863e5b60639806b05d34d9068b1c208ddd286bf201feffc461e2b62f320f.aa4e60601a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7659,7 +7659,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B196" sqref="B196"/>
+      <selection pane="bottomRight" activeCell="I386" sqref="I386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14106,7 +14106,7 @@
         <v>848</v>
       </c>
       <c r="K189" s="35" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="L189" s="37"/>
       <c r="M189" s="37"/>
@@ -20697,16 +20697,16 @@
         <v>792</v>
       </c>
       <c r="F382" s="23">
-        <v>45293</v>
+        <v>45309</v>
       </c>
       <c r="G382" s="24" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="I382" s="24" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>139</v>

</xml_diff>